<commit_message>
Added PRSB heading sections to spreadsheet
</commit_message>
<xml_diff>
--- a/docs/HelperFieldMappings.xlsx
+++ b/docs/HelperFieldMappings.xlsx
@@ -14,16 +14,17 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$2:$H$35</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$2:$H$44</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$2:$H$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$2:$H$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$2:$H$44</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$2:$H$44</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="147">
   <si>
     <t>Fields in RED can be ignored for a minimal document</t>
   </si>
@@ -401,6 +402,69 @@
   </si>
   <si>
     <t>TXT or B64</t>
+  </si>
+  <si>
+    <t>PRSB Sections</t>
+  </si>
+  <si>
+    <t>Admission Details</t>
+  </si>
+  <si>
+    <t>Individual Templates for each section</t>
+  </si>
+  <si>
+    <t>Allergies and Adverse Reaction</t>
+  </si>
+  <si>
+    <t>Assessment Scales</t>
+  </si>
+  <si>
+    <t>Clinical Details</t>
+  </si>
+  <si>
+    <t>Clinical Summary</t>
+  </si>
+  <si>
+    <t>Diagnoses</t>
+  </si>
+  <si>
+    <t>Discharge Details</t>
+  </si>
+  <si>
+    <t>Information Given</t>
+  </si>
+  <si>
+    <t>Investigations and Procedures Requested</t>
+  </si>
+  <si>
+    <t>Legal Information</t>
+  </si>
+  <si>
+    <t>Medications and Medical Devices</t>
+  </si>
+  <si>
+    <t>Participation in Research</t>
+  </si>
+  <si>
+    <t>Patient and Carer Concerns</t>
+  </si>
+  <si>
+    <t>Person Completing Record</t>
+  </si>
+  <si>
+    <t>Plan and Requested Actions</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t>Safety Alerts</t>
+  </si>
+  <si>
+    <t>Social Context</t>
+  </si>
+  <si>
+    <t>Special Requirements</t>
   </si>
 </sst>
 </file>
@@ -516,7 +580,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -525,7 +589,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -562,14 +626,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,19 +713,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -686,7 +750,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1650,7 +1714,7 @@
       </c>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
         <v>86</v>
       </c>
@@ -1668,7 +1732,7 @@
       </c>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
         <v>88</v>
       </c>
@@ -1688,7 +1752,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
         <v>89</v>
       </c>
@@ -1708,7 +1772,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
         <v>90</v>
       </c>
@@ -1726,7 +1790,7 @@
       </c>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
         <v>91</v>
       </c>
@@ -1744,7 +1808,7 @@
       </c>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="12" t="s">
         <v>92</v>
       </c>
@@ -1764,7 +1828,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
         <v>93</v>
       </c>
@@ -1782,7 +1846,7 @@
       </c>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="12" t="s">
         <v>94</v>
       </c>
@@ -1800,7 +1864,7 @@
       </c>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
         <v>96</v>
       </c>
@@ -1820,7 +1884,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
         <v>100</v>
       </c>
@@ -1838,7 +1902,7 @@
       </c>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
         <v>102</v>
       </c>
@@ -1856,7 +1920,7 @@
       </c>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
         <v>103</v>
       </c>
@@ -1874,7 +1938,7 @@
       </c>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
         <v>104</v>
       </c>
@@ -1892,7 +1956,7 @@
       </c>
       <c r="J59" s="8"/>
     </row>
-    <row r="60" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
         <v>105</v>
       </c>
@@ -1912,7 +1976,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
         <v>106</v>
       </c>
@@ -1930,7 +1994,7 @@
       </c>
       <c r="J61" s="8"/>
     </row>
-    <row r="62" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
         <v>107</v>
       </c>
@@ -1948,7 +2012,7 @@
       </c>
       <c r="J62" s="8"/>
     </row>
-    <row r="63" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
         <v>110</v>
       </c>
@@ -1966,7 +2030,7 @@
       </c>
       <c r="J63" s="8"/>
     </row>
-    <row r="64" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
         <v>112</v>
       </c>
@@ -1984,7 +2048,7 @@
       </c>
       <c r="J64" s="8"/>
     </row>
-    <row r="65" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8" t="s">
         <v>113</v>
       </c>
@@ -2004,7 +2068,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
         <v>115</v>
       </c>
@@ -2024,7 +2088,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8" t="s">
         <v>116</v>
       </c>
@@ -2042,7 +2106,7 @@
       </c>
       <c r="J67" s="8"/>
     </row>
-    <row r="68" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8" t="s">
         <v>117</v>
       </c>
@@ -2138,8 +2202,278 @@
         <v>125</v>
       </c>
     </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H76" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H87" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:H44"/>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
@@ -2150,7 +2484,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Started working on mappings from Kettering XML
</commit_message>
<xml_diff>
--- a/docs/HelperFieldMappings.xlsx
+++ b/docs/HelperFieldMappings.xlsx
@@ -1,30 +1,86 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="300" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="General" sheetId="1" r:id="rId1"/>
+    <sheet name="Kettering" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$2:$H$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$2:$H$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$2:$H$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$2:$H$44</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$2:$H$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">General!$A$2:$H$44</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">General!$A$2:$H$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">General!$A$2:$H$35</definedName>
+    <definedName name="Print_Area_0" localSheetId="0">General!$A$2:$H$35</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Emma Hatherly</author>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adam Hatherly:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Usually autogenerated, but can propagate from the Kettering XML</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F58" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adam Hatherly:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Small tweak to helper to use single point in time</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="241">
   <si>
     <t>Fields in RED can be ignored for a minimal document</t>
   </si>
@@ -465,15 +521,1080 @@
   </si>
   <si>
     <t>Special Requirements</t>
+  </si>
+  <si>
+    <t>&lt;MsgSender&gt;External System&lt;/MsgSender&gt;</t>
+  </si>
+  <si>
+    <t>&lt;MsgRecipient&gt;EDTS&lt;/MsgRecipient&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ServiceRequester&gt;&lt;IdValue&gt;1&lt;/IdValue&gt;&lt;/ServiceRequester&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ServiceProvider&gt;&lt;IdValue&gt;2&lt;/IdValue&gt;&lt;/ServiceProvider&gt;</t>
+  </si>
+  <si>
+    <t>&lt;PatientMatchingInfo&gt;</t>
+  </si>
+  <si>
+    <t>&lt;PatientId&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Id&gt;</t>
+  </si>
+  <si>
+    <t>&lt;IdType&gt;Nhs&lt;/IdType&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/Id&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/PatientId&gt;</t>
+  </si>
+  <si>
+    <t>&lt;PersonName_s&gt;</t>
+  </si>
+  <si>
+    <t>&lt;PersonNameType&gt;CU&lt;/PersonNameType&gt;</t>
+  </si>
+  <si>
+    <t>&lt;StructPersonName&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/StructPersonName&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/PersonName_s&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/PatientMatchingInfo&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Parties&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Party AgentId="1"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/Party&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Party AgentId="2"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/Parties&gt;</t>
+  </si>
+  <si>
+    <t>&lt;CodedData&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Term60/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Unit1/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ClinicalCode&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/CodedData&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ReportingInformation&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ReportingInformation&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ClinicalReport&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ReportContributor/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EventDateEnd/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;TextItem RcStatus="Current"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Cuid IdScope="Message"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;TextMarkupIndicator&gt;-//IETF//DTD HTML//EN&lt;/TextMarkupIndicator&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/TextBlock&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/TextItem&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ClinicalReport&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ReportMsg&gt;</t>
+  </si>
+  <si>
+    <t>Kettering XML</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Gap?</t>
+  </si>
+  <si>
+    <t>CDA Mapping</t>
+  </si>
+  <si>
+    <t>Urgency is not in the CDA spec?</t>
+  </si>
+  <si>
+    <t>In the distribution envelope that wraps the CDA</t>
+  </si>
+  <si>
+    <t>Mapped?</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>CDA Fields</t>
+  </si>
+  <si>
+    <t>documentID</t>
+  </si>
+  <si>
+    <t>Fixed? Discard</t>
+  </si>
+  <si>
+    <t>ITK DE</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ReportMsg MsgStatus="Live" MsgUrgency="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Normal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>" MsgRcptAckRequest="Always"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;MsgId&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>00000001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/MsgId&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;MsgIssueDate&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>200905031022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/MsgIssueDate&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;IdValue&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1542498716</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/IdValue&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Assume this will always be Nhs?</t>
+  </si>
+  <si>
+    <t>Add in enricher?</t>
+  </si>
+  <si>
+    <t>Generate?</t>
+  </si>
+  <si>
+    <t>Fixed?</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;FamilyName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BLOGGS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/FamilyName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;GivenName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>FREDERICK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/GivenName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BirthDate&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>19610831</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/BirthDate&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Sex&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/Sex&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;HcpCode IdType="GP"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>G2923343</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/HcpCode&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;HcpName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Young, C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/HcpName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;OrgCode IdType="PRA"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PCT1234</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/OrgCode&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;OrgName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Holmer Surgery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/OrgName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;LogicalAddress&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>urn:nhs-uk:addressing:ods:PCT1234</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/LogicalAddress&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;HcpCode IdType="Internal"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>NURS9003</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/HcpCode&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;HcpName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Maddocks, Sheila</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/HcpName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BossCode IdType="Specialist"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>C3524271</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/BossCode&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BossName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Siddiqi, Mashood</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/BossName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;DepartmentCode IdType="Internal"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3010</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/DepartmentCode&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;DepartmentName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Gastroenterology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/DepartmentName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;OrgCode IdType="Provider"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>REM00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/OrgCode&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;OrgName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>University Hospital Aintree</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/OrgName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ClinicalCode Type="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Read</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>" Schema="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;TermID&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/TermID&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Term30&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Serial peak expiratory flow rate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/Term30&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CodeName&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>339g.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/CodeName&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Value1&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/Value1&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ReportingReason&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/ReportingReason&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ReportingReferenceNumber&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>7268874342</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/ReportingReferenceNumber&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ActionRequested&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/ActionRequested&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;MedicationChanged&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/MedicationChanged&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ReportID&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>a88bb415-9294-4c13-bb92-eeb34c9f26c0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/ReportID&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ReportType&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Outpatient Letter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/ReportType&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ReportCode&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>GPLETTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/ReportCode&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ReportSourceType&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/ReportSourceType&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;EventDate&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>200609201030</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/EventDate&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;DocCreationDate&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>200609211233</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/DocCreationDate&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;TextBlock&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CDATA CONTENT</t>
+    </r>
+  </si>
+  <si>
+    <t>Need to check this is the right field to use?</t>
+  </si>
+  <si>
+    <t>nonXMLBody</t>
+  </si>
+  <si>
+    <t>eventEffectiveTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -481,21 +1602,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -511,15 +1617,34 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,118 +1663,75 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -708,49 +1790,343 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.7125506072874"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="15.3117408906883"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.9554655870445"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.5708502024291"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.8137651821862"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="63.2064777327935"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="38.7265625"/>
+    <col min="2" max="6" width="15.26953125"/>
+    <col min="7" max="7" width="11.90625"/>
+    <col min="8" max="8" width="35.54296875"/>
+    <col min="9" max="9" width="39.81640625"/>
+    <col min="10" max="10" width="63.1796875"/>
+    <col min="11" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -782,7 +2158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -806,7 +2182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -828,7 +2204,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -850,7 +2226,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -870,7 +2246,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -890,7 +2266,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -910,7 +2286,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -934,7 +2310,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -958,7 +2334,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -982,7 +2358,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
@@ -1006,7 +2382,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -1030,7 +2406,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
@@ -1052,7 +2428,7 @@
       </c>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -1072,7 +2448,7 @@
       </c>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
@@ -1092,7 +2468,7 @@
       </c>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>40</v>
       </c>
@@ -1114,7 +2490,7 @@
       </c>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1138,7 +2514,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10">
       <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
@@ -1158,7 +2534,7 @@
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10">
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
@@ -1178,7 +2554,7 @@
       </c>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10">
       <c r="A21" s="5" t="s">
         <v>45</v>
       </c>
@@ -1198,7 +2574,7 @@
       </c>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10">
       <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
@@ -1218,7 +2594,7 @@
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -1238,7 +2614,7 @@
       </c>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10">
       <c r="A24" s="5" t="s">
         <v>50</v>
       </c>
@@ -1258,7 +2634,7 @@
       </c>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10">
       <c r="A25" s="5" t="s">
         <v>51</v>
       </c>
@@ -1278,7 +2654,7 @@
       </c>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10">
       <c r="A26" s="5" t="s">
         <v>52</v>
       </c>
@@ -1302,7 +2678,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10">
       <c r="A27" s="5" t="s">
         <v>53</v>
       </c>
@@ -1324,7 +2700,7 @@
       </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10">
       <c r="A28" s="5" t="s">
         <v>54</v>
       </c>
@@ -1344,7 +2720,7 @@
       </c>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" s="10" customFormat="1">
       <c r="A29" s="8" t="s">
         <v>55</v>
       </c>
@@ -1364,7 +2740,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" s="10" customFormat="1">
       <c r="A30" s="8" t="s">
         <v>58</v>
       </c>
@@ -1384,7 +2760,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" s="10" customFormat="1">
       <c r="A31" s="8" t="s">
         <v>60</v>
       </c>
@@ -1402,7 +2778,7 @@
       </c>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10">
       <c r="A32" s="5" t="s">
         <v>61</v>
       </c>
@@ -1426,7 +2802,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10">
       <c r="A33" s="5" t="s">
         <v>63</v>
       </c>
@@ -1448,7 +2824,7 @@
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10">
       <c r="A34" s="5" t="s">
         <v>64</v>
       </c>
@@ -1472,7 +2848,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" s="10" customFormat="1">
       <c r="A35" s="8" t="s">
         <v>68</v>
       </c>
@@ -1492,7 +2868,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10">
       <c r="A36" s="11" t="s">
         <v>70</v>
       </c>
@@ -1514,7 +2890,7 @@
       </c>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10">
       <c r="A37" s="11" t="s">
         <v>72</v>
       </c>
@@ -1534,7 +2910,7 @@
       </c>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10">
       <c r="A38" s="11" t="s">
         <v>73</v>
       </c>
@@ -1554,7 +2930,7 @@
       </c>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10">
       <c r="A39" s="11" t="s">
         <v>74</v>
       </c>
@@ -1574,7 +2950,7 @@
       </c>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10">
       <c r="A40" s="11" t="s">
         <v>76</v>
       </c>
@@ -1598,7 +2974,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10">
       <c r="A41" s="11" t="s">
         <v>77</v>
       </c>
@@ -1620,7 +2996,7 @@
       </c>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10" s="10" customFormat="1">
       <c r="A42" s="8" t="s">
         <v>78</v>
       </c>
@@ -1640,7 +3016,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" s="10" customFormat="1">
       <c r="A43" s="8" t="s">
         <v>80</v>
       </c>
@@ -1660,7 +3036,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10" s="10" customFormat="1">
       <c r="A44" s="8" t="s">
         <v>81</v>
       </c>
@@ -1678,7 +3054,7 @@
       </c>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10" s="10" customFormat="1">
       <c r="A45" s="8" t="s">
         <v>82</v>
       </c>
@@ -1696,7 +3072,7 @@
       </c>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:10" s="10" customFormat="1">
       <c r="A46" s="8" t="s">
         <v>83</v>
       </c>
@@ -1714,7 +3090,7 @@
       </c>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:10">
       <c r="A47" s="12" t="s">
         <v>86</v>
       </c>
@@ -1732,7 +3108,7 @@
       </c>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>88</v>
       </c>
@@ -1752,7 +3128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:10">
       <c r="A49" s="12" t="s">
         <v>89</v>
       </c>
@@ -1772,7 +3148,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:10">
       <c r="A50" s="12" t="s">
         <v>90</v>
       </c>
@@ -1790,7 +3166,7 @@
       </c>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:10">
       <c r="A51" s="12" t="s">
         <v>91</v>
       </c>
@@ -1808,7 +3184,7 @@
       </c>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:10">
       <c r="A52" s="12" t="s">
         <v>92</v>
       </c>
@@ -1828,7 +3204,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:10">
       <c r="A53" s="12" t="s">
         <v>93</v>
       </c>
@@ -1846,7 +3222,7 @@
       </c>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:10">
       <c r="A54" s="12" t="s">
         <v>94</v>
       </c>
@@ -1864,7 +3240,7 @@
       </c>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:10">
       <c r="A55" s="8" t="s">
         <v>96</v>
       </c>
@@ -1884,7 +3260,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:10">
       <c r="A56" s="8" t="s">
         <v>100</v>
       </c>
@@ -1902,7 +3278,7 @@
       </c>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:10">
       <c r="A57" s="8" t="s">
         <v>102</v>
       </c>
@@ -1920,7 +3296,7 @@
       </c>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:10">
       <c r="A58" s="8" t="s">
         <v>103</v>
       </c>
@@ -1938,7 +3314,7 @@
       </c>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:10">
       <c r="A59" s="8" t="s">
         <v>104</v>
       </c>
@@ -1956,7 +3332,7 @@
       </c>
       <c r="J59" s="8"/>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:10">
       <c r="A60" s="8" t="s">
         <v>105</v>
       </c>
@@ -1976,7 +3352,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:10">
       <c r="A61" s="8" t="s">
         <v>106</v>
       </c>
@@ -1994,7 +3370,7 @@
       </c>
       <c r="J61" s="8"/>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:10">
       <c r="A62" s="8" t="s">
         <v>107</v>
       </c>
@@ -2012,7 +3388,7 @@
       </c>
       <c r="J62" s="8"/>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:10">
       <c r="A63" s="8" t="s">
         <v>110</v>
       </c>
@@ -2030,7 +3406,7 @@
       </c>
       <c r="J63" s="8"/>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:10">
       <c r="A64" s="8" t="s">
         <v>112</v>
       </c>
@@ -2048,7 +3424,7 @@
       </c>
       <c r="J64" s="8"/>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:10">
       <c r="A65" s="8" t="s">
         <v>113</v>
       </c>
@@ -2068,7 +3444,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:10">
       <c r="A66" s="8" t="s">
         <v>115</v>
       </c>
@@ -2088,7 +3464,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:10">
       <c r="A67" s="8" t="s">
         <v>116</v>
       </c>
@@ -2106,7 +3482,7 @@
       </c>
       <c r="J67" s="8"/>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:10">
       <c r="A68" s="8" t="s">
         <v>117</v>
       </c>
@@ -2124,7 +3500,7 @@
       </c>
       <c r="J68" s="8"/>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:10">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -2138,7 +3514,7 @@
       </c>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:10">
       <c r="A70" s="5" t="s">
         <v>119</v>
       </c>
@@ -2158,7 +3534,7 @@
       </c>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:10">
       <c r="A71" s="5" t="s">
         <v>121</v>
       </c>
@@ -2180,7 +3556,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:10">
       <c r="A72" s="5" t="s">
         <v>123</v>
       </c>
@@ -2202,274 +3578,274 @@
         <v>125</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:10">
       <c r="I73" s="14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:10">
+      <c r="A74" t="s">
         <v>127</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H74" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I74" s="0" t="s">
+      <c r="B74" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" t="s">
+        <v>14</v>
+      </c>
+      <c r="I74" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:10">
+      <c r="A75" t="s">
         <v>129</v>
       </c>
-      <c r="B75" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H75" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I75" s="0" t="s">
+      <c r="B75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:10">
+      <c r="A76" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H76" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I76" s="0" t="s">
+      <c r="B76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H76" t="s">
+        <v>14</v>
+      </c>
+      <c r="I76" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:10">
+      <c r="A77" t="s">
         <v>131</v>
       </c>
-      <c r="B77" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H77" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I77" s="0" t="s">
+      <c r="B77" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:10">
+      <c r="A78" t="s">
         <v>132</v>
       </c>
-      <c r="B78" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H78" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I78" s="0" t="s">
+      <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78" t="s">
+        <v>14</v>
+      </c>
+      <c r="I78" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
         <v>133</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H79" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I79" s="0" t="s">
+      <c r="B79" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" t="s">
+        <v>14</v>
+      </c>
+      <c r="I79" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:10">
+      <c r="A80" t="s">
         <v>134</v>
       </c>
-      <c r="B80" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H80" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I80" s="0" t="s">
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" t="s">
+        <v>14</v>
+      </c>
+      <c r="I80" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
         <v>135</v>
       </c>
-      <c r="B81" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H81" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I81" s="0" t="s">
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" t="s">
+        <v>14</v>
+      </c>
+      <c r="I81" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
         <v>136</v>
       </c>
-      <c r="B82" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I82" s="0" t="s">
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
         <v>137</v>
       </c>
-      <c r="B83" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I83" s="0" t="s">
+      <c r="B83" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
         <v>138</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H84" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I84" s="0" t="s">
+      <c r="B84" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
         <v>139</v>
       </c>
-      <c r="B85" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I85" s="0" t="s">
+      <c r="B85" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
         <v>140</v>
       </c>
-      <c r="B86" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H86" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I86" s="0" t="s">
+      <c r="B86" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
         <v>141</v>
       </c>
-      <c r="B87" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H87" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I87" s="0" t="s">
+      <c r="B87" t="s">
+        <v>13</v>
+      </c>
+      <c r="H87" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
         <v>142</v>
       </c>
-      <c r="B88" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H88" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I88" s="0" t="s">
+      <c r="B88" t="s">
+        <v>13</v>
+      </c>
+      <c r="H88" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="89" spans="1:9">
+      <c r="A89" t="s">
         <v>143</v>
       </c>
-      <c r="B89" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I89" s="0" t="s">
+      <c r="B89" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" t="s">
+        <v>14</v>
+      </c>
+      <c r="I89" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+    <row r="90" spans="1:9">
+      <c r="A90" t="s">
         <v>144</v>
       </c>
-      <c r="B90" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H90" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I90" s="0" t="s">
+      <c r="B90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+    <row r="91" spans="1:9">
+      <c r="A91" t="s">
         <v>145</v>
       </c>
-      <c r="B91" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H91" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I91" s="0" t="s">
+      <c r="B91" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+    <row r="92" spans="1:9">
+      <c r="A92" t="s">
         <v>146</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H92" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I92" s="0" t="s">
+      <c r="B92" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2477,64 +3853,1612 @@
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.440277777777778" right="0.359722222222222" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.44027777777777799" right="0.359722222222222" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1796875" customWidth="1"/>
+    <col min="6" max="6" width="36.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.54296875"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="1020" width="8.54296875"/>
   </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="F1" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="F10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="F11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="F12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="F14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="F16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="F17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="F18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="F19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="F20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="F21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="F22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="F23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="F24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="F25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="F26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="F27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="F28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="F29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="F30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="F31" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="F32" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="F33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" s="5"/>
+      <c r="M33" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="F34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L34" s="5"/>
+      <c r="M34" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="F35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="5"/>
+      <c r="M35" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="F36" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="F37" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="5"/>
+      <c r="M37" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="F38" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="F39" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" s="17"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="F40" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="F41" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" s="17"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L41" s="5"/>
+      <c r="M41" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="F42" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L42" s="5"/>
+      <c r="M42" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="F43" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" s="17"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="F44" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="17"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="F45" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="17"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="F46" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G46" s="17"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="F47" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G47" s="17"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="F48" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G48" s="17"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="F49" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G49" s="17"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="F50" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="17"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="F51" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G51" s="17"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="F52" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G52" s="17"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="F53" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="17"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="F54" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" s="17"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="F55" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G55" s="17"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="F56" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="F57" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G57" s="17"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="F58" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G58" s="17"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="F59" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G59" s="17"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="F60" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G60" s="17"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="F61" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G61" s="17"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="F62" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="F63" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G63" s="17"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="F64" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G64" s="17"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="F65" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G65" s="17"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="F66" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G66" s="17"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+      <c r="M66" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="F67" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67" s="17"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="F68" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G68" s="17"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="A78" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col min="1" max="1025" width="8.54296875"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>